<commit_message>
Final version of the integration of the two paths (see flowchart)
</commit_message>
<xml_diff>
--- a/data/overlap_analysis_dge_method.xlsx
+++ b/data/overlap_analysis_dge_method.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,11 +449,6 @@
           <t>Average overlap</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Lowest overlap</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -467,10 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>87.10889500363189</v>
-      </c>
-      <c r="D2" t="n">
-        <v>60</v>
+        <v>85.9731668718597</v>
       </c>
     </row>
     <row r="3">
@@ -485,10 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>33.8667427335943</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
+        <v>33.06992194236347</v>
       </c>
     </row>
     <row r="4">
@@ -503,10 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>32.57160911207178</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
+        <v>31.49790873184837</v>
       </c>
     </row>
   </sheetData>

</xml_diff>